<commit_message>
Fix issue with "Trenching" input to installation module. Replace incorrectly removed "ROV class" input. Add DateTimeDict for date outputs from installation module.
</commit_message>
<xml_diff>
--- a/test_data/installation/logisticsDB_equipment_python.xlsx
+++ b/test_data/installation/logisticsDB_equipment_python.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="810" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="810"/>
   </bookViews>
   <sheets>
     <sheet name="rov" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="N2" authorId="0" shapeId="0">
+    <comment ref="O2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0">
+    <comment ref="Q2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,30 +126,6 @@
           </rPr>
           <t xml:space="preserve">
 Including the payload of 400kg</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Original value from fugro probably too high compared to market rates. Discussions with  4C Offshore's subsea consultant Dr. Ron Haynes (who has a lot of experience managing subsea cable contracts) suggested £GBP11K more appropriate market rate for the spread, with reputable teams such as Fugro charging a premium</t>
         </r>
       </text>
     </comment>
@@ -173,11 +149,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 supervisor</t>
+Original value from fugro probably too high compared to market rates. Discussions with  4C Offshore's subsea consultant Dr. Ron Haynes (who has a lot of experience managing subsea cable contracts) suggested £GBP11K more appropriate market rate for the spread, with reputable teams such as Fugro charging a premium</t>
         </r>
       </text>
     </comment>
     <comment ref="P5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 supervisor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1073,7 +1073,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>Inspection class</t>
   </si>
@@ -1271,6 +1271,24 @@
   </si>
   <si>
     <t>Max Pile Mass</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Inspection class 1</t>
+  </si>
+  <si>
+    <t>Inspection class 2</t>
+  </si>
+  <si>
+    <t>Workclass 1</t>
+  </si>
+  <si>
+    <t>Workclass 2</t>
+  </si>
+  <si>
+    <t>Workclass 3</t>
   </si>
 </sst>
 </file>
@@ -2236,82 +2254,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125"/>
     <col min="2" max="2" width="17"/>
-    <col min="3" max="3" width="14.453125"/>
-    <col min="4" max="4" width="13.453125"/>
-    <col min="5" max="5" width="13.81640625"/>
-    <col min="6" max="6" width="13.453125"/>
-    <col min="7" max="7" width="12.26953125"/>
-    <col min="8" max="8" width="12.81640625"/>
-    <col min="9" max="9" width="14.81640625"/>
-    <col min="10" max="10" width="14.7265625"/>
-    <col min="11" max="11" width="11.7265625"/>
-    <col min="12" max="12" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875"/>
-    <col min="15" max="15" width="14.26953125"/>
-    <col min="16" max="16" width="13.81640625"/>
-    <col min="17" max="966" width="9.453125"/>
-    <col min="967" max="1019" width="8.54296875"/>
+    <col min="3" max="3" width="18.81640625" style="72" customWidth="1"/>
+    <col min="4" max="4" width="14.453125"/>
+    <col min="5" max="5" width="13.453125"/>
+    <col min="6" max="6" width="13.81640625"/>
+    <col min="7" max="7" width="13.453125"/>
+    <col min="8" max="8" width="12.26953125"/>
+    <col min="9" max="9" width="12.81640625"/>
+    <col min="10" max="10" width="14.81640625"/>
+    <col min="11" max="11" width="14.7265625"/>
+    <col min="12" max="12" width="11.7265625"/>
+    <col min="13" max="13" width="14.81640625" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875"/>
+    <col min="16" max="16" width="14.26953125"/>
+    <col min="17" max="17" width="13.81640625"/>
+    <col min="18" max="967" width="9.453125"/>
+    <col min="968" max="1020" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="47.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" ht="47.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
@@ -2322,254 +2343,270 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
-    </row>
-    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="AB1" s="3"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="54">
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="56">
+      <c r="D2" s="56">
         <v>1500</v>
       </c>
-      <c r="D2" s="56">
+      <c r="E2" s="56">
         <v>1.5</v>
       </c>
-      <c r="E2" s="56">
+      <c r="F2" s="56">
         <v>0.81499999999999995</v>
       </c>
-      <c r="F2" s="56">
+      <c r="G2" s="56">
         <v>0.60499999999999998</v>
       </c>
-      <c r="G2" s="56">
+      <c r="H2" s="56">
         <v>0.2</v>
       </c>
-      <c r="H2" s="56">
+      <c r="I2" s="56">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I2" s="56">
+      <c r="J2" s="56">
         <v>0</v>
       </c>
-      <c r="J2" s="57">
+      <c r="K2" s="57">
         <v>29.067099999999996</v>
       </c>
-      <c r="K2" s="57">
+      <c r="L2" s="57">
         <v>27.718</v>
-      </c>
-      <c r="L2" s="56">
-        <v>1</v>
       </c>
       <c r="M2" s="56">
         <v>1</v>
       </c>
-      <c r="N2" s="58">
+      <c r="N2" s="56">
+        <v>1</v>
+      </c>
+      <c r="O2" s="58">
         <v>2300</v>
       </c>
-      <c r="O2" s="58">
+      <c r="P2" s="58">
         <v>1370</v>
       </c>
-      <c r="P2" s="58">
+      <c r="Q2" s="58">
         <v>1250</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="59">
         <v>2</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="61">
+      <c r="D3" s="61">
         <v>2000</v>
       </c>
-      <c r="D3" s="61">
+      <c r="E3" s="61">
         <v>1.4</v>
       </c>
-      <c r="E3" s="61">
+      <c r="F3" s="61">
         <v>0.9</v>
       </c>
-      <c r="F3" s="61">
+      <c r="G3" s="61">
         <v>0.85</v>
       </c>
-      <c r="G3" s="61">
+      <c r="H3" s="61">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H3" s="61">
+      <c r="I3" s="61">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="I3" s="61">
+      <c r="J3" s="61">
         <v>890</v>
       </c>
-      <c r="J3" s="62">
+      <c r="K3" s="62">
         <v>28.2</v>
       </c>
-      <c r="K3" s="62">
+      <c r="L3" s="62">
         <v>22.5</v>
-      </c>
-      <c r="L3" s="61">
-        <v>1</v>
       </c>
       <c r="M3" s="61">
         <v>1</v>
       </c>
       <c r="N3" s="61">
+        <v>1</v>
+      </c>
+      <c r="O3" s="61">
         <v>2000</v>
       </c>
-      <c r="O3" s="61">
+      <c r="P3" s="61">
         <v>1900</v>
       </c>
-      <c r="P3" s="63">
+      <c r="Q3" s="63">
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="59">
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="61">
+      <c r="D4" s="61">
         <v>3000</v>
       </c>
-      <c r="D4" s="61">
+      <c r="E4" s="61">
         <v>2.59</v>
       </c>
-      <c r="E4" s="61">
+      <c r="F4" s="61">
         <v>1.4</v>
       </c>
-      <c r="F4" s="61">
+      <c r="G4" s="61">
         <v>1.8</v>
       </c>
-      <c r="G4" s="61">
+      <c r="H4" s="61">
         <v>2.54</v>
       </c>
-      <c r="H4" s="61">
+      <c r="I4" s="61">
         <v>0.22600000000000001</v>
       </c>
-      <c r="I4" s="61">
+      <c r="J4" s="61">
         <v>4092</v>
       </c>
-      <c r="J4" s="62">
+      <c r="K4" s="62">
         <v>82.9</v>
       </c>
-      <c r="K4" s="62">
+      <c r="L4" s="62">
         <v>66.400000000000006</v>
       </c>
-      <c r="L4" s="61">
+      <c r="M4" s="61">
         <v>1</v>
       </c>
-      <c r="M4" s="61">
+      <c r="N4" s="61">
         <v>2</v>
       </c>
-      <c r="N4" s="61">
+      <c r="O4" s="61">
         <v>5000</v>
       </c>
-      <c r="O4" s="61">
+      <c r="P4" s="61">
         <v>1900</v>
       </c>
-      <c r="P4" s="61">
+      <c r="Q4" s="61">
         <v>1800</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="59">
         <v>4</v>
       </c>
       <c r="B5" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="61">
+      <c r="D5" s="61">
         <v>3000</v>
       </c>
-      <c r="D5" s="61">
+      <c r="E5" s="61">
         <v>3.3149999999999999</v>
-      </c>
-      <c r="E5" s="61">
-        <v>1.73</v>
       </c>
       <c r="F5" s="61">
         <v>1.73</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="61">
+        <v>1.73</v>
+      </c>
+      <c r="H5" s="46">
         <v>4.2</v>
       </c>
-      <c r="H5" s="61">
+      <c r="I5" s="61">
         <v>0.4</v>
       </c>
-      <c r="I5" s="61">
+      <c r="J5" s="61">
         <v>4092</v>
       </c>
-      <c r="J5" s="62">
+      <c r="K5" s="62">
         <v>67.573999999999998</v>
       </c>
-      <c r="K5" s="62">
+      <c r="L5" s="62">
         <v>69.5</v>
       </c>
-      <c r="L5" s="61">
+      <c r="M5" s="61">
         <v>1</v>
       </c>
-      <c r="M5" s="61">
+      <c r="N5" s="61">
         <v>4</v>
       </c>
-      <c r="N5" s="46">
+      <c r="O5" s="46">
         <v>7000</v>
       </c>
-      <c r="O5" s="46">
+      <c r="P5" s="46">
         <v>2000</v>
       </c>
-      <c r="P5" s="46">
+      <c r="Q5" s="46">
         <v>1100</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="64">
         <v>5</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="66">
+      <c r="D6" s="66">
         <v>4000</v>
       </c>
-      <c r="D6" s="67">
+      <c r="E6" s="67">
         <v>3.2</v>
-      </c>
-      <c r="E6" s="67">
-        <v>1.8</v>
       </c>
       <c r="F6" s="67">
         <v>1.8</v>
       </c>
       <c r="G6" s="67">
+        <v>1.8</v>
+      </c>
+      <c r="H6" s="67">
         <v>3.5</v>
       </c>
-      <c r="H6" s="67">
+      <c r="I6" s="67">
         <v>0.25</v>
       </c>
-      <c r="I6" s="67">
+      <c r="J6" s="67">
         <v>4092</v>
       </c>
-      <c r="J6" s="68">
+      <c r="K6" s="68">
         <v>70</v>
       </c>
-      <c r="K6" s="68">
+      <c r="L6" s="68">
         <v>51</v>
       </c>
-      <c r="L6" s="67">
+      <c r="M6" s="67">
         <v>1</v>
       </c>
-      <c r="M6" s="67">
+      <c r="N6" s="67">
         <v>2</v>
       </c>
-      <c r="N6" s="67">
+      <c r="O6" s="67">
         <v>6000</v>
       </c>
-      <c r="O6" s="67">
+      <c r="P6" s="67">
         <v>1950</v>
       </c>
-      <c r="P6" s="67">
+      <c r="Q6" s="67">
         <v>1800</v>
       </c>
     </row>
@@ -2911,7 +2948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>